<commit_message>
Alteração de planilha de testes
</commit_message>
<xml_diff>
--- a/8RainhasAG.xlsx
+++ b/8RainhasAG.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cotriba\PycharmProjects\8puzzle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B3ACFB-98A9-4B9A-B8A3-C5D2F3C067FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAFD93F9-8B8D-4937-8714-8F2F8EB5E8CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6210" yWindow="3990" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="166">
   <si>
     <t>Solução encontrada em 203 gerações!</t>
   </si>
@@ -120,21 +120,6 @@
     <t>Solução encontrada em 913 gerações!</t>
   </si>
   <si>
-    <t>Alg Genético: Max Geração-&gt;1000||Mutação-&gt;0.05</t>
-  </si>
-  <si>
-    <t>35 sol</t>
-  </si>
-  <si>
-    <t>65 lim</t>
-  </si>
-  <si>
-    <t>97 sol</t>
-  </si>
-  <si>
-    <t>3 lim</t>
-  </si>
-  <si>
     <t>Solução encontrada em 977 gerações!</t>
   </si>
   <si>
@@ -360,9 +345,6 @@
     <t>Solução encontrada em 1337 gerações!</t>
   </si>
   <si>
-    <t>Alg Genético: Max Geração-&gt;2000||Mutação-&gt;0.5</t>
-  </si>
-  <si>
     <t>Solução encontrada em 717 gerações!</t>
   </si>
   <si>
@@ -537,13 +519,13 @@
     <t>Solução encontrada em 788 gerações!</t>
   </si>
   <si>
-    <t>81 sol</t>
-  </si>
-  <si>
-    <t>19 lim</t>
-  </si>
-  <si>
-    <t>Alg Genético: Max Geração-&gt;1500||Mutação-&gt;0.25</t>
+    <t>Alg Genético: Max Geração-&gt;1000||Mutação-&gt;0.05||35/100</t>
+  </si>
+  <si>
+    <t>Alg Genético: Max Geração-&gt;2000||Mutação-&gt;0.5||97/100</t>
+  </si>
+  <si>
+    <t>Alg Genético: Max Geração-&gt;1500||Mutação-&gt;0.25||81/100</t>
   </si>
 </sst>
 </file>
@@ -919,7 +901,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -933,34 +917,21 @@
     <col min="8" max="9" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" t="s">
-        <v>32</v>
-      </c>
+        <v>163</v>
+      </c>
+      <c r="B1" s="2"/>
       <c r="D1" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>34</v>
-      </c>
+        <v>164</v>
+      </c>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
       <c r="G1" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>170</v>
-      </c>
+        <v>165</v>
+      </c>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -968,12 +939,12 @@
       </c>
       <c r="B2" s="3"/>
       <c r="D2" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="5" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -984,12 +955,12 @@
       </c>
       <c r="B3" s="2"/>
       <c r="D3" s="5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="5" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
@@ -1000,7 +971,7 @@
       </c>
       <c r="B4" s="2"/>
       <c r="D4" s="5" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -1016,12 +987,12 @@
       </c>
       <c r="B5" s="2"/>
       <c r="D5" s="5" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="5" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
@@ -1032,7 +1003,7 @@
       </c>
       <c r="B6" s="3"/>
       <c r="D6" s="5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -1048,12 +1019,12 @@
       </c>
       <c r="B7" s="2"/>
       <c r="D7" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="5" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
@@ -1064,7 +1035,7 @@
       </c>
       <c r="B8" s="2"/>
       <c r="D8" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -1080,12 +1051,12 @@
       </c>
       <c r="B9" s="2"/>
       <c r="D9" s="5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="5" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
@@ -1096,12 +1067,12 @@
       </c>
       <c r="B10" s="2"/>
       <c r="D10" s="5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="5" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
@@ -1112,12 +1083,12 @@
       </c>
       <c r="B11" s="2"/>
       <c r="D11" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="5" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
@@ -1128,12 +1099,12 @@
       </c>
       <c r="B12" s="2"/>
       <c r="D12" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="5" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
@@ -1144,12 +1115,12 @@
       </c>
       <c r="B13" s="2"/>
       <c r="D13" s="5" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="5" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
@@ -1165,7 +1136,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="5" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
@@ -1176,12 +1147,12 @@
       </c>
       <c r="B15" s="2"/>
       <c r="D15" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="5" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -1192,7 +1163,7 @@
       </c>
       <c r="B16" s="2"/>
       <c r="D16" s="5" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -1208,7 +1179,7 @@
       </c>
       <c r="B17" s="2"/>
       <c r="D17" s="5" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
@@ -1224,7 +1195,7 @@
       </c>
       <c r="B18" s="2"/>
       <c r="D18" s="5" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
@@ -1240,12 +1211,12 @@
       </c>
       <c r="B19" s="2"/>
       <c r="D19" s="5" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="5" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
@@ -1256,12 +1227,12 @@
       </c>
       <c r="B20" s="2"/>
       <c r="D20" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="5" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
@@ -1272,12 +1243,12 @@
       </c>
       <c r="B21" s="2"/>
       <c r="D21" s="5" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="5" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
@@ -1293,7 +1264,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="5" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
@@ -1304,7 +1275,7 @@
       </c>
       <c r="B23" s="2"/>
       <c r="D23" s="5" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
@@ -1320,12 +1291,12 @@
       </c>
       <c r="B24" s="2"/>
       <c r="D24" s="5" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="5" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
@@ -1336,12 +1307,12 @@
       </c>
       <c r="B25" s="2"/>
       <c r="D25" s="5" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="5" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
@@ -1352,12 +1323,12 @@
       </c>
       <c r="B26" s="2"/>
       <c r="D26" s="5" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="5" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
@@ -1368,12 +1339,12 @@
       </c>
       <c r="B27" s="2"/>
       <c r="D27" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="5" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
@@ -1384,12 +1355,12 @@
       </c>
       <c r="B28" s="2"/>
       <c r="D28" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="5" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
@@ -1400,12 +1371,12 @@
       </c>
       <c r="B29" s="2"/>
       <c r="D29" s="5" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="5" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
@@ -1416,7 +1387,7 @@
       </c>
       <c r="B30" s="2"/>
       <c r="D30" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
@@ -1448,7 +1419,7 @@
       </c>
       <c r="B32" s="2"/>
       <c r="D32" s="5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
@@ -1464,7 +1435,7 @@
       </c>
       <c r="B33" s="2"/>
       <c r="D33" s="5" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
@@ -1480,12 +1451,12 @@
       </c>
       <c r="B34" s="2"/>
       <c r="D34" s="5" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
       <c r="G34" s="5" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
@@ -1496,7 +1467,7 @@
       </c>
       <c r="B35" s="2"/>
       <c r="D35" s="5" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
@@ -1512,7 +1483,7 @@
       </c>
       <c r="B36" s="2"/>
       <c r="D36" s="5" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
@@ -1528,12 +1499,12 @@
       </c>
       <c r="B37" s="2"/>
       <c r="D37" s="5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
       <c r="G37" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
@@ -1544,12 +1515,12 @@
       </c>
       <c r="B38" s="2"/>
       <c r="D38" s="5" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
       <c r="G38" s="5" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
@@ -1560,12 +1531,12 @@
       </c>
       <c r="B39" s="2"/>
       <c r="D39" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
       <c r="G39" s="5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
@@ -1576,12 +1547,12 @@
       </c>
       <c r="B40" s="2"/>
       <c r="D40" s="5" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
       <c r="G40" s="5" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
@@ -1597,7 +1568,7 @@
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
       <c r="G41" s="5" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
@@ -1608,12 +1579,12 @@
       </c>
       <c r="B42" s="2"/>
       <c r="D42" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
       <c r="G42" s="5" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
@@ -1624,12 +1595,12 @@
       </c>
       <c r="B43" s="2"/>
       <c r="D43" s="5" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
       <c r="G43" s="5" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
@@ -1640,12 +1611,12 @@
       </c>
       <c r="B44" s="2"/>
       <c r="D44" s="5" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
       <c r="G44" s="5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
@@ -1656,12 +1627,12 @@
       </c>
       <c r="B45" s="2"/>
       <c r="D45" s="5" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
       <c r="G45" s="5" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
@@ -1672,12 +1643,12 @@
       </c>
       <c r="B46" s="2"/>
       <c r="D46" s="5" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
       <c r="G46" s="5" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
@@ -1688,12 +1659,12 @@
       </c>
       <c r="B47" s="2"/>
       <c r="D47" s="5" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
       <c r="G47" s="5" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
@@ -1704,12 +1675,12 @@
       </c>
       <c r="B48" s="2"/>
       <c r="D48" s="5" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
       <c r="G48" s="5" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
@@ -1720,7 +1691,7 @@
       </c>
       <c r="B49" s="2"/>
       <c r="D49" s="5" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
@@ -1736,7 +1707,7 @@
       </c>
       <c r="B50" s="2"/>
       <c r="D50" s="5" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
@@ -1752,12 +1723,12 @@
       </c>
       <c r="B51" s="2"/>
       <c r="D51" s="5" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
       <c r="G51" s="5" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H51" s="2"/>
       <c r="I51" s="2"/>
@@ -1768,12 +1739,12 @@
       </c>
       <c r="B52" s="2"/>
       <c r="D52" s="5" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
       <c r="G52" s="5" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="H52" s="2"/>
       <c r="I52" s="2"/>
@@ -1784,12 +1755,12 @@
       </c>
       <c r="B53" s="2"/>
       <c r="D53" s="5" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
       <c r="G53" s="5" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="H53" s="2"/>
       <c r="I53" s="2"/>
@@ -1800,12 +1771,12 @@
       </c>
       <c r="B54" s="2"/>
       <c r="D54" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>
       <c r="G54" s="5" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="H54" s="2"/>
       <c r="I54" s="2"/>
@@ -1816,7 +1787,7 @@
       </c>
       <c r="B55" s="2"/>
       <c r="D55" s="5" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
@@ -1832,12 +1803,12 @@
       </c>
       <c r="B56" s="2"/>
       <c r="D56" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
       <c r="G56" s="5" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="H56" s="2"/>
       <c r="I56" s="2"/>
@@ -1848,12 +1819,12 @@
       </c>
       <c r="B57" s="2"/>
       <c r="D57" s="5" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
       <c r="G57" s="5" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="H57" s="2"/>
       <c r="I57" s="2"/>
@@ -1864,12 +1835,12 @@
       </c>
       <c r="B58" s="2"/>
       <c r="D58" s="5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
       <c r="G58" s="5" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H58" s="2"/>
       <c r="I58" s="2"/>
@@ -1880,12 +1851,12 @@
       </c>
       <c r="B59" s="2"/>
       <c r="D59" s="5" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
       <c r="G59" s="5" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="H59" s="2"/>
       <c r="I59" s="2"/>
@@ -1896,12 +1867,12 @@
       </c>
       <c r="B60" s="2"/>
       <c r="D60" s="5" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
       <c r="G60" s="5" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H60" s="2"/>
       <c r="I60" s="2"/>
@@ -1928,12 +1899,12 @@
       </c>
       <c r="B62" s="2"/>
       <c r="D62" s="5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
       <c r="G62" s="5" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H62" s="2"/>
       <c r="I62" s="2"/>
@@ -1944,7 +1915,7 @@
       </c>
       <c r="B63" s="2"/>
       <c r="D63" s="5" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
@@ -1960,12 +1931,12 @@
       </c>
       <c r="B64" s="2"/>
       <c r="D64" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
       <c r="G64" s="5" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="H64" s="2"/>
       <c r="I64" s="2"/>
@@ -1976,12 +1947,12 @@
       </c>
       <c r="B65" s="2"/>
       <c r="D65" s="5" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
       <c r="G65" s="5" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H65" s="2"/>
       <c r="I65" s="2"/>
@@ -1992,12 +1963,12 @@
       </c>
       <c r="B66" s="2"/>
       <c r="D66" s="5" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
       <c r="G66" s="5" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="H66" s="2"/>
       <c r="I66" s="2"/>
@@ -2008,12 +1979,12 @@
       </c>
       <c r="B67" s="2"/>
       <c r="D67" s="5" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="E67" s="2"/>
       <c r="F67" s="2"/>
       <c r="G67" s="5" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="H67" s="2"/>
       <c r="I67" s="2"/>
@@ -2024,12 +1995,12 @@
       </c>
       <c r="B68" s="2"/>
       <c r="D68" s="5" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E68" s="2"/>
       <c r="F68" s="2"/>
       <c r="G68" s="5" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H68" s="2"/>
       <c r="I68" s="2"/>
@@ -2040,7 +2011,7 @@
       </c>
       <c r="B69" s="2"/>
       <c r="D69" s="5" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E69" s="2"/>
       <c r="F69" s="2"/>
@@ -2056,12 +2027,12 @@
       </c>
       <c r="B70" s="2"/>
       <c r="D70" s="5" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E70" s="2"/>
       <c r="F70" s="2"/>
       <c r="G70" s="5" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="H70" s="2"/>
       <c r="I70" s="2"/>
@@ -2072,12 +2043,12 @@
       </c>
       <c r="B71" s="2"/>
       <c r="D71" s="5" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
       <c r="G71" s="5" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="H71" s="2"/>
       <c r="I71" s="2"/>
@@ -2088,12 +2059,12 @@
       </c>
       <c r="B72" s="2"/>
       <c r="D72" s="5" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E72" s="2"/>
       <c r="F72" s="2"/>
       <c r="G72" s="5" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="H72" s="2"/>
       <c r="I72" s="2"/>
@@ -2104,12 +2075,12 @@
       </c>
       <c r="B73" s="2"/>
       <c r="D73" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E73" s="2"/>
       <c r="F73" s="2"/>
       <c r="G73" s="5" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H73" s="2"/>
       <c r="I73" s="2"/>
@@ -2120,12 +2091,12 @@
       </c>
       <c r="B74" s="2"/>
       <c r="D74" s="5" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E74" s="2"/>
       <c r="F74" s="2"/>
       <c r="G74" s="5" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="H74" s="2"/>
       <c r="I74" s="2"/>
@@ -2136,12 +2107,12 @@
       </c>
       <c r="B75" s="2"/>
       <c r="D75" s="5" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E75" s="2"/>
       <c r="F75" s="2"/>
       <c r="G75" s="5" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="H75" s="2"/>
       <c r="I75" s="2"/>
@@ -2152,12 +2123,12 @@
       </c>
       <c r="B76" s="2"/>
       <c r="D76" s="5" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E76" s="2"/>
       <c r="F76" s="2"/>
       <c r="G76" s="5" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="H76" s="2"/>
       <c r="I76" s="2"/>
@@ -2168,12 +2139,12 @@
       </c>
       <c r="B77" s="2"/>
       <c r="D77" s="5" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E77" s="2"/>
       <c r="F77" s="2"/>
       <c r="G77" s="5" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="H77" s="2"/>
       <c r="I77" s="2"/>
@@ -2200,7 +2171,7 @@
       </c>
       <c r="B79" s="2"/>
       <c r="D79" s="5" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E79" s="2"/>
       <c r="F79" s="2"/>
@@ -2216,12 +2187,12 @@
       </c>
       <c r="B80" s="2"/>
       <c r="D80" s="5" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E80" s="2"/>
       <c r="F80" s="2"/>
       <c r="G80" s="5" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="H80" s="2"/>
       <c r="I80" s="2"/>
@@ -2232,12 +2203,12 @@
       </c>
       <c r="B81" s="2"/>
       <c r="D81" s="5" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E81" s="2"/>
       <c r="F81" s="2"/>
       <c r="G81" s="5" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="H81" s="2"/>
       <c r="I81" s="2"/>
@@ -2248,12 +2219,12 @@
       </c>
       <c r="B82" s="2"/>
       <c r="D82" s="5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E82" s="2"/>
       <c r="F82" s="2"/>
       <c r="G82" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="H82" s="2"/>
       <c r="I82" s="2"/>
@@ -2269,7 +2240,7 @@
       <c r="E83" s="2"/>
       <c r="F83" s="2"/>
       <c r="G83" s="5" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="H83" s="2"/>
       <c r="I83" s="2"/>
@@ -2280,7 +2251,7 @@
       </c>
       <c r="B84" s="2"/>
       <c r="D84" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E84" s="2"/>
       <c r="F84" s="2"/>
@@ -2296,7 +2267,7 @@
       </c>
       <c r="B85" s="2"/>
       <c r="D85" s="5" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E85" s="2"/>
       <c r="F85" s="2"/>
@@ -2312,12 +2283,12 @@
       </c>
       <c r="B86" s="2"/>
       <c r="D86" s="5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E86" s="2"/>
       <c r="F86" s="2"/>
       <c r="G86" s="5" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="H86" s="2"/>
       <c r="I86" s="2"/>
@@ -2328,12 +2299,12 @@
       </c>
       <c r="B87" s="2"/>
       <c r="D87" s="5" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="E87" s="2"/>
       <c r="F87" s="2"/>
       <c r="G87" s="5" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="H87" s="2"/>
       <c r="I87" s="2"/>
@@ -2344,12 +2315,12 @@
       </c>
       <c r="B88" s="2"/>
       <c r="D88" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E88" s="2"/>
       <c r="F88" s="2"/>
       <c r="G88" s="5" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="H88" s="2"/>
       <c r="I88" s="2"/>
@@ -2360,7 +2331,7 @@
       </c>
       <c r="B89" s="2"/>
       <c r="D89" s="5" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E89" s="2"/>
       <c r="F89" s="2"/>
@@ -2376,12 +2347,12 @@
       </c>
       <c r="B90" s="2"/>
       <c r="D90" s="5" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E90" s="2"/>
       <c r="F90" s="2"/>
       <c r="G90" s="5" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="H90" s="2"/>
       <c r="I90" s="2"/>
@@ -2392,12 +2363,12 @@
       </c>
       <c r="B91" s="2"/>
       <c r="D91" s="5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E91" s="2"/>
       <c r="F91" s="2"/>
       <c r="G91" s="5" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="H91" s="2"/>
       <c r="I91" s="2"/>
@@ -2408,12 +2379,12 @@
       </c>
       <c r="B92" s="2"/>
       <c r="D92" s="5" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E92" s="2"/>
       <c r="F92" s="2"/>
       <c r="G92" s="5" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="H92" s="2"/>
       <c r="I92" s="2"/>
@@ -2424,12 +2395,12 @@
       </c>
       <c r="B93" s="2"/>
       <c r="D93" s="5" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E93" s="2"/>
       <c r="F93" s="2"/>
       <c r="G93" s="5" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="H93" s="2"/>
       <c r="I93" s="2"/>
@@ -2440,12 +2411,12 @@
       </c>
       <c r="B94" s="2"/>
       <c r="D94" s="5" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E94" s="2"/>
       <c r="F94" s="2"/>
       <c r="G94" s="5" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H94" s="2"/>
       <c r="I94" s="2"/>
@@ -2456,12 +2427,12 @@
       </c>
       <c r="B95" s="2"/>
       <c r="D95" s="5" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E95" s="2"/>
       <c r="F95" s="2"/>
       <c r="G95" s="5" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="H95" s="2"/>
       <c r="I95" s="2"/>
@@ -2472,12 +2443,12 @@
       </c>
       <c r="B96" s="2"/>
       <c r="D96" s="5" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E96" s="2"/>
       <c r="F96" s="2"/>
       <c r="G96" s="5" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="H96" s="2"/>
       <c r="I96" s="2"/>
@@ -2488,12 +2459,12 @@
       </c>
       <c r="B97" s="2"/>
       <c r="D97" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E97" s="2"/>
       <c r="F97" s="2"/>
       <c r="G97" s="5" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="H97" s="2"/>
       <c r="I97" s="2"/>
@@ -2504,12 +2475,12 @@
       </c>
       <c r="B98" s="2"/>
       <c r="D98" s="5" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E98" s="2"/>
       <c r="F98" s="2"/>
       <c r="G98" s="5" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="H98" s="2"/>
       <c r="I98" s="2"/>
@@ -2520,12 +2491,12 @@
       </c>
       <c r="B99" s="2"/>
       <c r="D99" s="5" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E99" s="2"/>
       <c r="F99" s="2"/>
       <c r="G99" s="5" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="H99" s="2"/>
       <c r="I99" s="2"/>
@@ -2536,12 +2507,12 @@
       </c>
       <c r="B100" s="2"/>
       <c r="D100" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E100" s="2"/>
       <c r="F100" s="2"/>
       <c r="G100" s="5" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="H100" s="2"/>
       <c r="I100" s="2"/>
@@ -2552,12 +2523,12 @@
       </c>
       <c r="B101" s="2"/>
       <c r="D101" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E101" s="2"/>
       <c r="F101" s="2"/>
       <c r="G101" s="5" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="H101" s="2"/>
       <c r="I101" s="2"/>

</xml_diff>